<commit_message>
dry run new simple
</commit_message>
<xml_diff>
--- a/FlaskEventSchedulerApp/slipstream_event_schedule.xlsx
+++ b/FlaskEventSchedulerApp/slipstream_event_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://slipstreaminc2-my.sharepoint.com/personal/bbartling_slipstreaminc_org/Documents/Desktop/hvac_volttron_agents/FlaskEventSchedulerApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{7C0967D9-3BB8-4872-80CB-CBCB081312FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6EBC3F7A-F4B6-474F-92DA-BC8F6B6B6CEE}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{7C0967D9-3BB8-4872-80CB-CBCB081312FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1B32A429-4915-4F0A-B817-DAA13C1AAFB7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -888,7 +888,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>44461</v>
+        <v>44462</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>44461.010416666664</v>
+        <v>44462.010416666664</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>44461.020833333336</v>
+        <v>44462.020833333336</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>44461.03125</v>
+        <v>44462.03125</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>44461.041666666664</v>
+        <v>44462.041666666664</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>44461.052083333336</v>
+        <v>44462.052083333336</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -936,7 +936,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>44461.0625</v>
+        <v>44462.0625</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>44461.072916666664</v>
+        <v>44462.072916666664</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>44461.083333333336</v>
+        <v>44462.083333333336</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>44461.09375</v>
+        <v>44462.09375</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>44461.104166666664</v>
+        <v>44462.104166666664</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>44461.114583333336</v>
+        <v>44462.114583333336</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>44461.125</v>
+        <v>44462.125</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>44461.135416666664</v>
+        <v>44462.135416666664</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>44461.145833333336</v>
+        <v>44462.145833333336</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>44461.15625</v>
+        <v>44462.15625</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>44461.166666666664</v>
+        <v>44462.166666666664</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44461.177083333336</v>
+        <v>44462.177083333336</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44461.1875</v>
+        <v>44462.1875</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>44461.197916666664</v>
+        <v>44462.197916666664</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>44461.208333333336</v>
+        <v>44462.208333333336</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>44461.21875</v>
+        <v>44462.21875</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>44461.229166666664</v>
+        <v>44462.229166666664</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>44461.239583333336</v>
+        <v>44462.239583333336</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>44461.25</v>
+        <v>44462.25</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>44461.260416666664</v>
+        <v>44462.260416666664</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>44461.270833333336</v>
+        <v>44462.270833333336</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>44461.28125</v>
+        <v>44462.28125</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>44461.291666666664</v>
+        <v>44462.291666666664</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>44461.302083333336</v>
+        <v>44462.302083333336</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>44461.3125</v>
+        <v>44462.3125</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>44461.322916666664</v>
+        <v>44462.322916666664</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>44461.333333333336</v>
+        <v>44462.333333333336</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>44461.34375</v>
+        <v>44462.34375</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1160,39 +1160,39 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>44461.354166666664</v>
+        <v>44462.354166666664</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>44461.364583333336</v>
+        <v>44462.364583333336</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>44461.375</v>
+        <v>44462.375</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>44461.385416666664</v>
+        <v>44462.385416666664</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>44461.395833333336</v>
+        <v>44462.395833333336</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>44461.40625</v>
+        <v>44462.40625</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>44461.416666666664</v>
+        <v>44462.416666666664</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>44461.427083333336</v>
+        <v>44462.427083333336</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>44461.4375</v>
+        <v>44462.4375</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>44461.447916666664</v>
+        <v>44462.447916666664</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>44461.458333333336</v>
+        <v>44462.458333333336</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>44461.46875</v>
+        <v>44462.46875</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>44461.479166666664</v>
+        <v>44462.479166666664</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>44461.489583333336</v>
+        <v>44462.489583333336</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>44461.5</v>
+        <v>44462.5</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>44461.510416666664</v>
+        <v>44462.510416666664</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>44461.520833333336</v>
+        <v>44462.520833333336</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>44461.53125</v>
+        <v>44462.53125</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>44461.541666666664</v>
+        <v>44462.541666666664</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>44461.552083333336</v>
+        <v>44462.552083333336</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>44461.5625</v>
+        <v>44462.5625</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>44461.572916666664</v>
+        <v>44462.572916666664</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>44461.583333333336</v>
+        <v>44462.583333333336</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>44461.59375</v>
+        <v>44462.59375</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>44461.604166666664</v>
+        <v>44462.604166666664</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -1360,7 +1360,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <v>44461.614583333336</v>
+        <v>44462.614583333336</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>44461.625</v>
+        <v>44462.625</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -1376,7 +1376,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <v>44461.635416666664</v>
+        <v>44462.635416666664</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <v>44461.645833333336</v>
+        <v>44462.645833333336</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>44461.65625</v>
+        <v>44462.65625</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>44461.666666666664</v>
+        <v>44462.666666666664</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -1408,7 +1408,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>44461.677083333336</v>
+        <v>44462.677083333336</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>44461.6875</v>
+        <v>44462.6875</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>44461.697916666664</v>
+        <v>44462.697916666664</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>44461.708333333336</v>
+        <v>44462.708333333336</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>44461.71875</v>
+        <v>44462.71875</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <v>44461.729166666664</v>
+        <v>44462.729166666664</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <v>44461.739583333336</v>
+        <v>44462.739583333336</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <v>44461.75</v>
+        <v>44462.75</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>44461.760416666664</v>
+        <v>44462.760416666664</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>44461.770833333336</v>
+        <v>44462.770833333336</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>44461.78125</v>
+        <v>44462.78125</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>44461.791666666664</v>
+        <v>44462.791666666664</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>44461.802083333336</v>
+        <v>44462.802083333336</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>44461.8125</v>
+        <v>44462.8125</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>44461.822916666664</v>
+        <v>44462.822916666664</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>44461.833333333336</v>
+        <v>44462.833333333336</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>44461.84375</v>
+        <v>44462.84375</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>44461.854166666664</v>
+        <v>44462.854166666664</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <v>44461.864583333336</v>
+        <v>44462.864583333336</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <v>44461.875</v>
+        <v>44462.875</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>44461.885416666664</v>
+        <v>44462.885416666664</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <v>44461.895833333336</v>
+        <v>44462.895833333336</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <v>44461.90625</v>
+        <v>44462.90625</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <v>44461.916666666664</v>
+        <v>44462.916666666664</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <v>44461.927083333336</v>
+        <v>44462.927083333336</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>44461.9375</v>
+        <v>44462.9375</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>44461.947916666664</v>
+        <v>44462.947916666664</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
-        <v>44461.958333333336</v>
+        <v>44462.958333333336</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
-        <v>44461.96875</v>
+        <v>44462.96875</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
-        <v>44461.979166666664</v>
+        <v>44462.979166666664</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
-        <v>44461.989583333336</v>
+        <v>44462.989583333336</v>
       </c>
       <c r="B97">
         <v>0</v>

</xml_diff>